<commit_message>
Cambio de tipo de dato Route
</commit_message>
<xml_diff>
--- a/Service.Catalog/wwwroot/layout/excel/company/CompañiaFormulario.xlsx
+++ b/Service.Catalog/wwwroot/layout/excel/company/CompañiaFormulario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lapaxsis-00\source\repos\API\Service.Catalog\wwwroot\layout\excel\company\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lapaxsis-00\source\repos\Nueva carpeta\Service.Catalog\wwwroot\layout\excel\company\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F797D5B1-1A23-4900-B330-60FBC038334F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42BF76A8-11DE-4356-AF35-8E9FE6CD9F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{3229E258-B22D-4941-8A9E-0DA32DA258DE}"/>
+    <workbookView xWindow="1905" yWindow="195" windowWidth="14865" windowHeight="10875" xr2:uid="{3229E258-B22D-4941-8A9E-0DA32DA258DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Compañias" sheetId="1" r:id="rId1"/>
@@ -148,9 +148,6 @@
     <t>{{Compañias.NombreComercial}}</t>
   </si>
   <si>
-    <t>{{Compañias.ListaPrecioId}}</t>
-  </si>
-  <si>
     <t>{{Compañias.PromocionesId}}</t>
   </si>
   <si>
@@ -218,6 +215,9 @@
   </si>
   <si>
     <t>{{Compañias.ProcedenciaId}}</t>
+  </si>
+  <si>
+    <t>{{Compañias.PrecioListaId}}</t>
   </si>
 </sst>
 </file>
@@ -298,17 +298,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -682,7 +682,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:C11"/>
+      <selection activeCell="B13" sqref="B13:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,27 +691,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="117" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="7"/>
+      <c r="C3" s="6"/>
       <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -721,15 +721,15 @@
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="7"/>
+      <c r="C5" s="6"/>
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -739,15 +739,15 @@
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="7"/>
+      <c r="C7" s="6"/>
       <c r="D7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -757,15 +757,15 @@
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="7"/>
+      <c r="C9" s="6"/>
       <c r="D9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -775,15 +775,15 @@
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="7"/>
+      <c r="B11" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="6"/>
       <c r="D11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -793,15 +793,15 @@
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="7"/>
+      <c r="B13" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="6"/>
       <c r="D13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -811,15 +811,15 @@
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="7"/>
+      <c r="B15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="6"/>
       <c r="D15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -829,15 +829,15 @@
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="7"/>
+      <c r="B17" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="6"/>
       <c r="D17" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -848,7 +848,7 @@
         <v>17</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -859,7 +859,7 @@
         <v>18</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -870,7 +870,7 @@
         <v>19</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -878,24 +878,24 @@
         <v>20</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26" s="8"/>
+      <c r="A26" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="5"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>3</v>
@@ -904,30 +904,30 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="C29" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="D29" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B9:C9"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B11:C11"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>